<commit_message>
thêm 3 testcase bài học vào trong testCase.xlsx.
</commit_message>
<xml_diff>
--- a/9. Test Document/TestCase.xlsx
+++ b/9. Test Document/TestCase.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -361,6 +361,33 @@
   </si>
   <si>
     <t>Dữ liệu tuần 12 bị mất</t>
+  </si>
+  <si>
+    <t>FUNC_BaiHoc_TC1</t>
+  </si>
+  <si>
+    <t>Chọn bài học và hiển thị nội dung bài học</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chọn tuần 1 . Chọn bài học tập đọc . Chọn bài Mẹ Ốm. </t>
+  </si>
+  <si>
+    <t>Khi chọn tuần 1 , màn hình hiện ra các bài học thuộc tuần 1 : tập đọc , tập làm văn , luyện từ và câu , chính tả , kể chuyện. Sau khi chọn tập đọc thì màn hình sẽ hiện ra hai bài tập đọc : Dế mèn bênh vực kẻ yếu và bài Mẹ Ốm. Sau khi click chọn bài Mẹ Ốm thì màn hình sẽ hiện ra nội dung bài Mẹ Ốm: " Mọi hôm mẹ thích vui chơi..."</t>
+  </si>
+  <si>
+    <t>FUNC_BaiHoc_TC2</t>
+  </si>
+  <si>
+    <t>Chọn tuần 1 . Chọn bài học tập đọc . Trở lai màn hình trước đó. Chọn bài học chính tả.</t>
+  </si>
+  <si>
+    <t>Khi chọn tuần 1 , màn hình hiện ra các bài học thuộc tuần 1 : tập đọc , tập làm văn , luyện từ và câu , chính tả , kể chuyện. Sau khi chọn tập đọc thì màn hình sẽ hiện ra hai bài tập đọc : Dế mèn bênh vực kẻ yếu và bài Mẹ Ốm. Trở về màn hình trước đó , chọn bài học chính tả.</t>
+  </si>
+  <si>
+    <t>FUNC_BaiHoc_TC3</t>
+  </si>
+  <si>
+    <t>Chọn tuần học 1 . Chọn bài học chính tả. Chọn bài mẹ ốm . Trở lại màn hính chính.</t>
   </si>
 </sst>
 </file>
@@ -429,7 +456,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -452,11 +479,107 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -477,19 +600,420 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H13" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="A1:H13"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="TestCase ID" dataDxfId="7"/>
+    <tableColumn id="2" name="Chức Năng Kiểm Tra" dataDxfId="6"/>
+    <tableColumn id="3" name="Giả Định" dataDxfId="5"/>
+    <tableColumn id="4" name="Dữ Liệu Dùng Để Kiểm Tra" dataDxfId="4"/>
+    <tableColumn id="5" name="Các Bước Thực Hiện" dataDxfId="3"/>
+    <tableColumn id="6" name="Kết Quả Mong Đợi" dataDxfId="2"/>
+    <tableColumn id="7" name="Kết Quả Thực Hiện" dataDxfId="1"/>
+    <tableColumn id="8" name="Ghi Chú" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -777,53 +1301,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K7:K11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="27.83203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.83203125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="30.1640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="36.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="25.83203125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="29.6640625" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="9.33203125" style="2"/>
+    <col min="1" max="1" width="27.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="36.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="9.28515625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="57.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="18" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" ht="90">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -841,15 +1365,15 @@
       <c r="F2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" ht="232.5" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -867,13 +1391,13 @@
       <c r="F3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="5"/>
+      <c r="H3" s="14"/>
     </row>
-    <row r="4" spans="1:8" ht="293.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:8" ht="255">
+      <c r="A4" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -891,15 +1415,15 @@
       <c r="F4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="191.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:8" ht="153">
+      <c r="A5" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -917,12 +1441,13 @@
       <c r="F5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>34</v>
       </c>
+      <c r="H5" s="14"/>
     </row>
     <row r="6" spans="1:8" ht="114.75">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -940,15 +1465,15 @@
       <c r="F6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="14" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="5" customFormat="1" ht="114.75">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="12" t="s">
         <v>31</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -966,19 +1491,97 @@
       <c r="F7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="E9" s="3"/>
+    <row r="8" spans="1:8" ht="102">
+      <c r="A8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="89.25">
+      <c r="A9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="38.25">
+      <c r="A10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="11"/>
+      <c r="H11" s="14"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="11"/>
+      <c r="H12" s="14"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="19"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="7" orientation="portrait" verticalDpi="0" copies="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -988,7 +1591,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1000,7 +1603,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Thêm 6 testcase Giải trí trong TestCase.xlsx.
</commit_message>
<xml_diff>
--- a/9. Test Document/TestCase.xlsx
+++ b/9. Test Document/TestCase.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="69">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -389,12 +389,78 @@
   <si>
     <t>Chọn tuần học 1 . Chọn bài học chính tả. Chọn bài mẹ ốm . Trở lại màn hính chính.</t>
   </si>
+  <si>
+    <t>FUNC_GiaiTri_TC1</t>
+  </si>
+  <si>
+    <t>Chọn chức năng giải trí</t>
+  </si>
+  <si>
+    <t>Chọn chức năng giải trí từ màn hình chính.</t>
+  </si>
+  <si>
+    <t>Khi chọn chức năng giải trí màn hình sẽ hiện ra các trò chơi giải trí để lựa chọn: chơi game , đố vui , nhật ký</t>
+  </si>
+  <si>
+    <t>FUNC_GiaiTri_TC2</t>
+  </si>
+  <si>
+    <t>Chọn trò chơi giải trí Đố vui</t>
+  </si>
+  <si>
+    <t>Chọn trò chơi giải trí từ màn hình chính. Chọn trò chơi Đố vui</t>
+  </si>
+  <si>
+    <t>Khi chọn trò chơi giải trí từ màn hình chính . Màn hình sẽ hiện ra các trò chơi cho mình lựa chọn : nhật ký , đố vui , chơi game. Khi chọn trò chơi đố vui , màn hình sẽ hiện ra trò chơi đố vui</t>
+  </si>
+  <si>
+    <t>FUNC_GiaiTri_TC3</t>
+  </si>
+  <si>
+    <t>Chọn trò chơi game</t>
+  </si>
+  <si>
+    <t>Chọn trò chơi giải trí từ màn hình chính. Chọn trò chơi game</t>
+  </si>
+  <si>
+    <t>Khi chọn trò chơi giải trí từ màn hình chính . Màn hình sẽ hiện ra các trò chơi cho mình lựa chọn : nhật ký , đố vui , chơi game. Khi chọn trò chơi game màn hình sẽ hiện ra trò chơi game</t>
+  </si>
+  <si>
+    <t>Chọn Nhật ký để giải trí</t>
+  </si>
+  <si>
+    <t>Chọn trò chơi giải trí từ màn hình chính. Chọn Nhật Ký</t>
+  </si>
+  <si>
+    <t>Khi chọn trò chơi giải trí từ màn hình chính . Màn hình sẽ hiện ra các trò chơi cho mình lựa chọn : nhật ký , đố vui , chơi game. Khi chọn Nhật Ký màn hình sẽ  hiện ra những gì liên quan đến Nhật Ký.</t>
+  </si>
+  <si>
+    <t>FUNC_GiaiTri_TC4</t>
+  </si>
+  <si>
+    <t>FUNC_GiaiTri_TC5</t>
+  </si>
+  <si>
+    <t>Trở lại màn hình trước đó để chọn trò giải trí khác</t>
+  </si>
+  <si>
+    <t>Chọn Giải trí từ màn hình chính. Chọn trò chơi game . Trở lại màn hính trước đó . Chọn trò đố vui để giải trí.</t>
+  </si>
+  <si>
+    <t>Khi chọn giải trí từ màn hình chính , màn hình sẽ hiện ra các trò giải trí để lựa chọn : nhật ký , chơi game , đố vui. Khi chọn trò chơi game màn hình hiện ra trò chơi game. Trở lại màn hình trước đó . Chọn trò chơi đố vui , màn hình hiện ra trò chơi đố vui.</t>
+  </si>
+  <si>
+    <t>FUNC_GiaiTri_TC6</t>
+  </si>
+  <si>
+    <t>Chọn trò chơi giải trí từ màn hình chính. Chọn trò chơi game . Trờ lại màn hình chính</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -441,6 +507,16 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -579,7 +655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -631,19 +707,20 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1000,8 +1077,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H13" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
-  <autoFilter ref="A1:H13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H16" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="A1:H16"/>
   <tableColumns count="8">
     <tableColumn id="1" name="TestCase ID" dataDxfId="7"/>
     <tableColumn id="2" name="Chức Năng Kiểm Tra" dataDxfId="6"/>
@@ -1301,10 +1378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
@@ -1314,7 +1391,7 @@
     <col min="3" max="3" width="17.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="24.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="30.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="36.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="44.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="25.85546875" style="8" customWidth="1"/>
     <col min="8" max="8" width="29.7109375" style="5" customWidth="1"/>
     <col min="9" max="16384" width="9.28515625" style="2"/>
@@ -1346,7 +1423,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="6" customFormat="1" ht="90">
+    <row r="2" spans="1:8" s="6" customFormat="1" ht="65.25">
       <c r="A2" s="9" t="s">
         <v>8</v>
       </c>
@@ -1498,7 +1575,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="102">
+    <row r="8" spans="1:8" ht="76.5">
       <c r="A8" s="5" t="s">
         <v>38</v>
       </c>
@@ -1511,14 +1588,14 @@
       <c r="D8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="19" t="s">
         <v>40</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="89.25">
+    <row r="9" spans="1:8" ht="63.75">
       <c r="A9" s="5" t="s">
         <v>42</v>
       </c>
@@ -1558,23 +1635,134 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="11"/>
+    <row r="11" spans="1:8" ht="25.5">
+      <c r="A11" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="11"/>
+    <row r="12" spans="1:8" ht="51">
+      <c r="A12" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="H12" s="14"/>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="19"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="23"/>
+    <row r="13" spans="1:8" ht="51">
+      <c r="A13" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="14"/>
+    </row>
+    <row r="14" spans="1:8" ht="51">
+      <c r="A14" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="22"/>
+      <c r="H14" s="23"/>
+    </row>
+    <row r="15" spans="1:8" ht="63.75">
+      <c r="A15" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="22"/>
+      <c r="H15" s="23"/>
+    </row>
+    <row r="16" spans="1:8" ht="38.25">
+      <c r="A16" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="22"/>
+      <c r="H16" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Thêm 5 testcase Nhật Ký trong TestCase.xlsx
</commit_message>
<xml_diff>
--- a/9. Test Document/TestCase.xlsx
+++ b/9. Test Document/TestCase.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="88">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -454,6 +454,63 @@
   </si>
   <si>
     <t>Chọn trò chơi giải trí từ màn hình chính. Chọn trò chơi game . Trờ lại màn hình chính</t>
+  </si>
+  <si>
+    <t>FUNC_NhatKy_TC1</t>
+  </si>
+  <si>
+    <t>Chọn Giải Trí Nhật Ký</t>
+  </si>
+  <si>
+    <t>Khi chọn chức năng giải trí từ màn hình chính . Màn hình sẽ hiện ra các trò chơi giải trí cho mình lựa chọn: nhật ký , game , đố vui. Chọn Nhật Ký. Hiện ra màn hình có liên quan đến Nhật Ký</t>
+  </si>
+  <si>
+    <t>FUNC_NhatKy_TC2</t>
+  </si>
+  <si>
+    <t>Viết nhật ký</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chọn  Giải Trí từ màn hình chính. Chọn Nhật Ký. </t>
+  </si>
+  <si>
+    <t>Khi chọn chức năng giải trí màn hình sẽ hiện ra các trò chơi giải trí để lựa chọn : chơi game , nhật ký , đố vui. Chọn Nhật ký . Màn hình hiện ra cửa số cho mình ghi pass. Nếu ghi pass đúng thì sẽ hiện ra màn hình cho mình ghi nhật ký.</t>
+  </si>
+  <si>
+    <t>FUNC_NhatKy_TC3</t>
+  </si>
+  <si>
+    <t>Lưu nhật ký</t>
+  </si>
+  <si>
+    <t>Chọn chức năng giải trí từ màn hình chính. Chọn Nhật Ký để giải trí . Ghi pass , Viết nhật ký.</t>
+  </si>
+  <si>
+    <t>Chọn chức năng giải trí từ màn hình , chọn nhật ký , ghi pass , viết nhật ký , lưu đoạn nhật ký vừa ghi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khi chọn chức năng giải trí thì màn hình hiện ra dánh sách các trò giải trí: nhật ký , chơi game , đố vui. Khi chọn nhật ký thì màn hình sẽ hiện ra cửa sổ để ghi pass . Nếu ghi đúng pass , hiện ra màn hình để ghi nhật ký . Trước khi thoát khỏi nhật ký thì có thông báo lưu lại đoạn nhật ký vừa ghi hay không . </t>
+  </si>
+  <si>
+    <t>Khi chọn chức năng giải trí thì màn hình hiện ra danh sách các trò giải trí: nhật ký , chơi game , đố vui. Khi chọn nhật ký thì màn hình sẽ hiện ra cửa sổ để ghi pass . Nếu ghi đúng pass , không ghi pass , trở lại màn hình trước đó.</t>
+  </si>
+  <si>
+    <t>Trở lại màn hình trước đó</t>
+  </si>
+  <si>
+    <t>Chọn chức năng giải trí từ màn hình , chọn nhật ký , trở lại màn hình trước đó .</t>
+  </si>
+  <si>
+    <t>FUNC_NhatKy_TC4</t>
+  </si>
+  <si>
+    <t>FUNC_NhatKy_TC5</t>
+  </si>
+  <si>
+    <t>Chọn chức năng giải trí từ màn hình , chọn nhật ký , trở lại màn hình chính của phần mềm</t>
+  </si>
+  <si>
+    <t>Trở lại màn hình chính của phần mềm bất cứ lúc nào.</t>
   </si>
 </sst>
 </file>
@@ -1077,8 +1134,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H16" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
-  <autoFilter ref="A1:H16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H21" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="A1:H21"/>
   <tableColumns count="8">
     <tableColumn id="1" name="TestCase ID" dataDxfId="7"/>
     <tableColumn id="2" name="Chức Năng Kiểm Tra" dataDxfId="6"/>
@@ -1378,10 +1435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
@@ -1763,6 +1820,115 @@
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="23"/>
+    </row>
+    <row r="17" spans="1:8" ht="51">
+      <c r="A17" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17" s="22"/>
+      <c r="H17" s="23"/>
+    </row>
+    <row r="18" spans="1:8" ht="63.75">
+      <c r="A18" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19" spans="1:8" ht="76.5">
+      <c r="A19" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="G19" s="22"/>
+      <c r="H19" s="23"/>
+    </row>
+    <row r="20" spans="1:8" ht="63.75">
+      <c r="A20" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="22"/>
+      <c r="H20" s="23"/>
+    </row>
+    <row r="21" spans="1:8" ht="38.25">
+      <c r="A21" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="22"/>
+      <c r="H21" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Thêm testcase tập đọc và luyện từ và câu
</commit_message>
<xml_diff>
--- a/9. Test Document/TestCase.xlsx
+++ b/9. Test Document/TestCase.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="108">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -511,6 +511,88 @@
   </si>
   <si>
     <t>Trở lại màn hình chính của phần mềm bất cứ lúc nào.</t>
+  </si>
+  <si>
+    <t>FUNC_TapDoc_TC1</t>
+  </si>
+  <si>
+    <t>Chọn tuần 5, click vào phần tập đọc.
+- Trở về trang trước.
+- Chọn tuần 35, phần tập đọc</t>
+  </si>
+  <si>
+    <t>FUNC_TapDoc_TC2</t>
+  </si>
+  <si>
+    <t>Trả lời trắc nghiệm
+Hiển thị và thông báo kết quả</t>
+  </si>
+  <si>
+    <t>Chọn tuần 15, chức năng tập đọc
+- Chọn câu hỏi cuối cùng.
+- Chọn đáp án c.
+- Chọn đáp án b.
+- Chọn chức năng xem kết quả.</t>
+  </si>
+  <si>
+    <t>Ở câu hỏi cuối cùng của tuần 15 phần tập đọc, chỉ được chọn một đáp án. Sau khi chọn đáp c, chọn lại đáp án b, thì đáp án c bị huỷ chọn.
+- Hiển thị kết quả là đáp án b.</t>
+  </si>
+  <si>
+    <t>FUNC_TapDoc_TC3</t>
+  </si>
+  <si>
+    <t>Qua câu hỏi kế tiếp.
+Lùi lại câu hỏi trước đó.
+Trở về màn hình chính</t>
+  </si>
+  <si>
+    <t>Chọn tuần 15, chức năng tập đọc
+- Chọn câu hỏi trước đó.
+- Click qua câu hỏi tiếp theo.
+- Click qua câu hỏi tiếp theo.
+- Click qua câu hỏi tiếp theo.
+- Trở lại màn hình chính</t>
+  </si>
+  <si>
+    <t>Khi vừa mới chọn chức năng tập đọc của tuần 15, chức năng chọn câu hỏi trước không hiển thị vì đây là câu hỏi đầu tiên.
+- Khi click qua câu hỏi tiếp theo thì hiển thị cả 2 chức năng chọn câu hỏi trước và câu hỏi tiếp theo.
+- Khi click qua câu hỏi kế tiếp nữa thì không hiển thị chức năng chọn câu hỏi kế tiếp, vì đây là câu hỏi cuối.</t>
+  </si>
+  <si>
+    <t>FUNC_TapDoc_TC4</t>
+  </si>
+  <si>
+    <t>Hướng dẫn học</t>
+  </si>
+  <si>
+    <t>Chọn tuần 6
+- Chọn chức năng học tập đọc</t>
+  </si>
+  <si>
+    <t>Khi vừa chọn chức năng tập đọc của tuần 6, màn hình xuất hiện hướng dẫn học sinh cách thức học phần học tập đọc này.</t>
+  </si>
+  <si>
+    <t>FUNC_LuyenTuCau_TC1</t>
+  </si>
+  <si>
+    <t>Chọn tuần 13, bài luyện từ và câu.
+- Trở lại màn hình trước
+- Chọn tuần 6, bài luyện từ và câu thứ 2</t>
+  </si>
+  <si>
+    <t>FUNC_LuyenTuCau_TC2</t>
+  </si>
+  <si>
+    <t>Trả lời trắc nghiệm</t>
+  </si>
+  <si>
+    <t>Khi học tập đọc tuần 5, màn hình hiển thị phần bài học tập đọc của tuần 5. cụ thể bài "Những hạt thóc giống".
+Không thể chọn phần tập đọc của tuần 35 được, vì không có dữ liệu</t>
+  </si>
+  <si>
+    <t>Khi chọn bài luyện từ và câu tuần 13, màn hình hiển thị bài học: "Mở rộng vốn từ: Ý chí - Nghị lực"
+- Chọn bài luyện từ và câu thứ 2 của tuần 6, màn hình hiển thị bài học: "Mở rộng vốn từ: Trung thực - Tự trọng".</t>
   </si>
 </sst>
 </file>
@@ -712,7 +794,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -778,6 +860,33 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1134,8 +1243,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H21" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
-  <autoFilter ref="A1:H21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H27" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="A1:H27"/>
   <tableColumns count="8">
     <tableColumn id="1" name="TestCase ID" dataDxfId="7"/>
     <tableColumn id="2" name="Chức Năng Kiểm Tra" dataDxfId="6"/>
@@ -1435,10 +1544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
@@ -1929,6 +2038,134 @@
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="23"/>
+    </row>
+    <row r="22" spans="1:8" ht="51">
+      <c r="A22" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="F22" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="G22" s="28"/>
+      <c r="H22" s="29"/>
+    </row>
+    <row r="23" spans="1:8" ht="63.75">
+      <c r="A23" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="G23" s="28"/>
+      <c r="H23" s="29"/>
+    </row>
+    <row r="24" spans="1:8" ht="89.25">
+      <c r="A24" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="G24" s="28"/>
+      <c r="H24" s="29"/>
+    </row>
+    <row r="25" spans="1:8" ht="38.25">
+      <c r="A25" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="G25" s="28"/>
+      <c r="H25" s="29"/>
+    </row>
+    <row r="26" spans="1:8" ht="63.75">
+      <c r="A26" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="G26" s="28"/>
+      <c r="H26" s="29"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="32"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>